<commit_message>
Upload versão para teste.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://t2cconsultoria365-my.sharepoint.com/personal/marcelo_thieme_t2cconsultoria_com_br/Documents/Documentos/UiPath/prj_integracao_MarceloThieme/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{51A9A92A-B7FC-47DA-9FC9-936E08C2E9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F6024A5-42A0-4789-B042-20672C586814}"/>
   <bookViews>
-    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -88,78 +88,115 @@
   </si>
   <si>
     <t>Framework</t>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>Queue_ExtracaoCidadesSulMG_ColetaDados_IBGE</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator. (Lista de Cidades do Sul de Minas Gerais para a busca das respectivas informações do site do IBGE.)</t>
+  </si>
+  <si>
+    <t>https://cidades.ibge.gov.br/brasil/mg/</t>
+  </si>
+  <si>
+    <t>URL_SiteCidadesMG_IBGE</t>
+  </si>
+  <si>
+    <t>URL_SiteBuscaCEP_Correios</t>
+  </si>
+  <si>
+    <t>https://buscacepinter.correios.com.br/app/faixa_cep_uf_localidade/index.php</t>
+  </si>
+  <si>
+    <t>URL do site dos Correios para buscar os CEPs por estado.</t>
+  </si>
+  <si>
+    <t>URL_IBGE</t>
+  </si>
+  <si>
+    <t>https://cidades.ibge.gov.br/</t>
+  </si>
+  <si>
+    <t>URL principal do IBGE.</t>
+  </si>
+  <si>
+    <t>Pasta_Output</t>
+  </si>
+  <si>
+    <t>C:\Users\marcelo.thieme\OneDrive - T2C CONSULTORIA LTDA\Documentos\UiPath\prj_integracao_MarceloThieme\Data\Output</t>
+  </si>
+  <si>
+    <t>Pasta Output para a gravação dos arquivos gerados pelo robô.</t>
+  </si>
+  <si>
+    <t>URL do site do IBGE para buscar informações das Cidades de Minas Gerais.</t>
   </si>
 </sst>
 </file>
@@ -177,6 +214,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -211,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -221,6 +259,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -239,7 +278,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -538,7 +577,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -585,22 +624,24 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -612,17 +653,57 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1619,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1670,21 +1751,21 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1789,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1811,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1822,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1833,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2802,7 +2883,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Melhorias conforme relatório Inspector.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://t2cconsultoria365-my.sharepoint.com/personal/marcelo_thieme_t2cconsultoria_com_br/Documents/Documentos/UiPath/prj_integracao_MarceloThieme/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{51A9A92A-B7FC-47DA-9FC9-936E08C2E9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F6024A5-42A0-4789-B042-20672C586814}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{51A9A92A-B7FC-47DA-9FC9-936E08C2E9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B86B23C9-6130-41CA-9BB8-72A34CAE5150}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -190,13 +190,22 @@
     <t>Pasta_Output</t>
   </si>
   <si>
-    <t>C:\Users\marcelo.thieme\OneDrive - T2C CONSULTORIA LTDA\Documentos\UiPath\prj_integracao_MarceloThieme\Data\Output</t>
-  </si>
-  <si>
-    <t>Pasta Output para a gravação dos arquivos gerados pelo robô.</t>
-  </si>
-  <si>
     <t>URL do site do IBGE para buscar informações das Cidades de Minas Gerais.</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>Estado_Pesquisa_CEP</t>
+  </si>
+  <si>
+    <t>Informar o estado que deseja efetuar a pesquisa dos CEPs. OBS.: Utilizar sempre a sigla do estado desejado.</t>
+  </si>
+  <si>
+    <t>Pasta Output para a gravação dos arquivos gerados pelo robô. Caso necessário utilizar o endereço completo da pasta Output.</t>
+  </si>
+  <si>
+    <t>Data\Output</t>
   </si>
 </sst>
 </file>
@@ -574,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -671,41 +680,51 @@
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="2" t="s">
         <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" t="s">
-        <v>53</v>
+        <v>47</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>54</v>
+      <c r="A13" t="s">
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -1689,6 +1708,8 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>